<commit_message>
Add process cooling to demand model and archetypes database
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/C/Users/User/Documents/GitHub/CityEnergyAnalyst/cea/databases/SIN/archetypes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/GitHub/CityEnergyAnalyst/cea/databases/SG/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBBA1BA-9BEA-AE46-A454-C41CC845EEE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26800" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19600" tabRatio="785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId4"/>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="75">
   <si>
     <t>Code</t>
   </si>
@@ -253,16 +254,19 @@
   </si>
   <si>
     <t>Es</t>
+  </si>
+  <si>
+    <t>Qcpro_Wm2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1134,17 +1138,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
@@ -1159,7 +1163,7 @@
     <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
@@ -1215,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1272,7 +1276,7 @@
       </c>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1664,7 +1668,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1776,7 +1780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -2290,14 +2294,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="12" customWidth="1"/>
@@ -2309,7 +2313,7 @@
     <col min="8" max="8" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
@@ -2335,7 +2339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -2361,7 +2365,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -2413,7 +2417,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -2439,7 +2443,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -2465,7 +2469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -2517,7 +2521,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -2543,7 +2547,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="7" t="s">
         <v>66</v>
       </c>
@@ -2569,7 +2573,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -2595,7 +2599,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -2621,7 +2625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -2647,7 +2651,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -2673,7 +2677,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -2751,7 +2755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -2777,7 +2781,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -2803,7 +2807,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="8:8">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -2838,14 +2842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="12" customWidth="1"/>
@@ -2858,7 +2862,7 @@
     <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
@@ -2887,7 +2891,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -2916,7 +2920,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -2945,7 +2949,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -3003,7 +3007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -3061,7 +3065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3090,7 +3094,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -3119,7 +3123,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="7" t="s">
         <v>66</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -3177,7 +3181,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -3206,7 +3210,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -3235,7 +3239,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -3264,7 +3268,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -3293,7 +3297,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -3322,7 +3326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -3380,7 +3384,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -3409,7 +3413,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="8:8">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -3451,14 +3455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
@@ -3469,7 +3473,7 @@
     <col min="7" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3495,7 +3499,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -3521,7 +3525,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -3573,7 +3577,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -3599,7 +3603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -3625,7 +3629,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -3651,7 +3655,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3678,7 +3682,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
@@ -3730,7 +3734,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -3756,7 +3760,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -3808,7 +3812,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -3834,7 +3838,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -3860,7 +3864,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -3886,7 +3890,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -3912,7 +3916,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -3939,7 +3943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -3965,7 +3969,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -3998,14 +4002,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.33203125" style="1" customWidth="1"/>
@@ -4014,12 +4018,12 @@
     <col min="6" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4048,13 +4052,16 @@
         <v>16</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -4088,8 +4095,11 @@
       <c r="K2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -4123,8 +4133,11 @@
       <c r="K3" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -4158,8 +4171,11 @@
       <c r="K4" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -4193,8 +4209,11 @@
       <c r="K5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -4228,8 +4247,11 @@
       <c r="K6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -4263,8 +4285,11 @@
       <c r="K7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -4298,8 +4323,11 @@
       <c r="K8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -4333,8 +4361,11 @@
       <c r="K9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
@@ -4368,8 +4399,11 @@
       <c r="K10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -4403,8 +4437,11 @@
       <c r="K11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -4438,8 +4475,11 @@
       <c r="K12" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -4473,8 +4513,11 @@
       <c r="K13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -4508,8 +4551,11 @@
       <c r="K14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -4543,8 +4589,11 @@
       <c r="K15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -4578,8 +4627,11 @@
       <c r="K16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -4608,13 +4660,16 @@
         <v>0</v>
       </c>
       <c r="J17" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K17" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -4651,8 +4706,11 @@
       <c r="K18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -4686,8 +4744,11 @@
       <c r="K19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -4719,6 +4780,9 @@
         <v>0</v>
       </c>
       <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
erase setpoints form construction database
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/GitHub/CityEnergyAnalyst/cea/databases/SG/archetypes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBBA1BA-9BEA-AE46-A454-C41CC845EEE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19600" tabRatio="785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId4"/>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="71">
   <si>
     <t>Code</t>
   </si>
@@ -58,9 +57,6 @@
     <t>Ve_lps</t>
   </si>
   <si>
-    <t>Ths_set_C</t>
-  </si>
-  <si>
     <t>X_ghp</t>
   </si>
   <si>
@@ -76,9 +72,6 @@
     <t>Qs_Wp</t>
   </si>
   <si>
-    <t>Tcs_set_C</t>
-  </si>
-  <si>
     <t>Vww_lpd</t>
   </si>
   <si>
@@ -131,12 +124,6 @@
   </si>
   <si>
     <t>Ed_Wm2</t>
-  </si>
-  <si>
-    <t>Tcs_setb_C</t>
-  </si>
-  <si>
-    <t>Ths_setb_C</t>
   </si>
   <si>
     <t>type_win</t>
@@ -262,11 +249,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1138,7 +1125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
@@ -1148,89 +1135,89 @@
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="7" width="7.1640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="10.83203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
+    <col min="5" max="7" width="7.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="10.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3">
         <v>0.9</v>
@@ -1257,37 +1244,37 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3">
         <v>0.9</v>
@@ -1314,36 +1301,36 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3">
         <v>0.9</v>
@@ -1370,36 +1357,36 @@
         <v>0.35</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
@@ -1426,36 +1413,36 @@
         <v>0.59</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3">
         <v>0.9</v>
@@ -1482,36 +1469,36 @@
         <v>0.59</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E7" s="3">
         <v>0.9</v>
@@ -1538,36 +1525,36 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3">
         <v>0.9</v>
@@ -1594,36 +1581,36 @@
         <v>0.59</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3">
         <v>0.9</v>
@@ -1650,36 +1637,36 @@
         <v>0.1</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3">
         <v>0.9</v>
@@ -1706,36 +1693,36 @@
         <v>0.35</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3">
         <v>0.9</v>
@@ -1762,36 +1749,36 @@
         <v>0.35</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E12" s="3">
         <v>0.9</v>
@@ -1818,36 +1805,36 @@
         <v>0.35</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="3">
         <v>0.9</v>
@@ -1874,36 +1861,36 @@
         <v>0.35</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3">
         <v>0.9</v>
@@ -1930,36 +1917,36 @@
         <v>0.35</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E15" s="3">
         <v>0.9</v>
@@ -1986,36 +1973,36 @@
         <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E16" s="3">
         <v>0.9</v>
@@ -2042,36 +2029,36 @@
         <v>0.5</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3">
         <v>0.9</v>
@@ -2098,36 +2085,36 @@
         <v>0</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3">
         <v>0.9</v>
@@ -2154,36 +2141,36 @@
         <v>0.35</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3">
         <v>0.9</v>
@@ -2210,36 +2197,36 @@
         <v>0.35</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="3">
         <v>0.9</v>
@@ -2266,22 +2253,22 @@
         <v>0.35</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2294,37 +2281,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="4"/>
-    <col min="6" max="6" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="4"/>
-    <col min="8" max="8" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="4"/>
+    <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="4"/>
+    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2336,504 +2323,504 @@
         <v>3</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
+      <c r="H4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
+      <c r="B13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
+      <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="6" t="s">
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -2842,38 +2829,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" style="4"/>
-    <col min="7" max="7" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2888,561 +2875,561 @@
         <v>5</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="G8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="I8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="I9" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="I11" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="G12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="G13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="I13" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="G14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="I14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="I15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="G17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="I17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="G18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="I18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="G19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="I19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="G20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -3455,543 +3442,299 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5">
+        <v>30</v>
+      </c>
+      <c r="D5" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="C6" s="5">
+        <v>30</v>
+      </c>
+      <c r="D6" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="8">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" ref="B8" si="0">111*0.15+10*0.85</f>
+        <v>25.15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5">
+        <v>30</v>
+      </c>
+      <c r="D13" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="5">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5">
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="5">
+        <f>B9</f>
+        <v>31</v>
+      </c>
+      <c r="C18" s="5">
+        <v>30</v>
+      </c>
+      <c r="D18" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="8">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="C19" s="5">
+        <v>30</v>
+      </c>
+      <c r="D19" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5">
         <v>10</v>
       </c>
-      <c r="F2" s="5">
-        <v>10</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="C20" s="5">
         <v>30</v>
       </c>
-      <c r="H2" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="8">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8">
-        <v>27</v>
-      </c>
-      <c r="E3" s="5">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5">
-        <v>10</v>
-      </c>
-      <c r="G3" s="5">
-        <v>30</v>
-      </c>
-      <c r="H3" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="8">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5">
-        <v>10</v>
-      </c>
-      <c r="D4" s="8">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5">
-        <v>30</v>
-      </c>
-      <c r="H4" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="8">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3">
-        <v>37</v>
-      </c>
-      <c r="E5" s="5">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5">
-        <v>30</v>
-      </c>
-      <c r="H5" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="8">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3">
-        <v>37</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5">
-        <v>30</v>
-      </c>
-      <c r="H6" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="8">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5">
-        <v>10</v>
-      </c>
-      <c r="D7" s="8">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5">
-        <v>30</v>
-      </c>
-      <c r="H7" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3">
-        <v>37</v>
-      </c>
-      <c r="E8" s="5">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
-        <v>25.15</v>
-      </c>
-      <c r="G8" s="5">
-        <v>30</v>
-      </c>
-      <c r="H8" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="8">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5">
-        <v>31</v>
-      </c>
-      <c r="G9" s="5">
-        <v>30</v>
-      </c>
-      <c r="H9" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="8">
-        <v>24</v>
-      </c>
-      <c r="C10" s="5">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3">
-        <v>37</v>
-      </c>
-      <c r="E10" s="5">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5">
-        <v>30</v>
-      </c>
-      <c r="H10" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="8">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3">
-        <v>37</v>
-      </c>
-      <c r="E11" s="5">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5">
-        <v>8</v>
-      </c>
-      <c r="G11" s="5">
-        <v>30</v>
-      </c>
-      <c r="H11" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
-      </c>
-      <c r="D12" s="8">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5">
-        <v>10</v>
-      </c>
-      <c r="F12" s="5">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5">
-        <v>30</v>
-      </c>
-      <c r="H12" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3">
-        <v>37</v>
-      </c>
-      <c r="E13" s="5">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5">
-        <v>10</v>
-      </c>
-      <c r="G13" s="5">
-        <v>30</v>
-      </c>
-      <c r="H13" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="8">
-        <v>50</v>
-      </c>
-      <c r="C14" s="5">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5">
-        <v>50</v>
-      </c>
-      <c r="E14" s="5">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5">
-        <v>36</v>
-      </c>
-      <c r="G14" s="5">
-        <v>30</v>
-      </c>
-      <c r="H14" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="8">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
-      </c>
-      <c r="D15" s="8">
-        <v>24</v>
-      </c>
-      <c r="E15" s="5">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5">
-        <v>36</v>
-      </c>
-      <c r="G15" s="5">
-        <v>30</v>
-      </c>
-      <c r="H15" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="8">
-        <v>50</v>
-      </c>
-      <c r="C16" s="5">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5">
-        <v>10</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>30</v>
-      </c>
-      <c r="H16" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8">
-        <v>-5</v>
-      </c>
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
-      <c r="D17" s="8">
-        <v>-5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>10</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>30</v>
-      </c>
-      <c r="H17" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="8">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3">
-        <v>37</v>
-      </c>
-      <c r="E18" s="5">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5">
-        <f>F9</f>
-        <v>31</v>
-      </c>
-      <c r="G18" s="5">
-        <v>30</v>
-      </c>
-      <c r="H18" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="8">
-        <v>24</v>
-      </c>
-      <c r="C19" s="5">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3">
-        <v>37</v>
-      </c>
-      <c r="E19" s="5">
-        <v>10</v>
-      </c>
-      <c r="F19" s="5">
-        <v>10</v>
-      </c>
-      <c r="G19" s="5">
-        <v>30</v>
-      </c>
-      <c r="H19" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="8">
-        <v>24</v>
-      </c>
-      <c r="C20" s="5">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3">
-        <v>37</v>
-      </c>
-      <c r="E20" s="5">
-        <v>10</v>
-      </c>
-      <c r="F20" s="5">
-        <v>10</v>
-      </c>
-      <c r="G20" s="5">
-        <v>30</v>
-      </c>
-      <c r="H20" s="5">
+      <c r="D20" s="5">
         <v>70</v>
       </c>
     </row>
@@ -4002,68 +3745,68 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="B2" s="8">
         <v>70</v>
@@ -4099,9 +3842,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5">
         <v>70</v>
@@ -4137,9 +3880,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>70</v>
@@ -4175,9 +3918,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="8">
         <v>70</v>
@@ -4213,9 +3956,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="8">
         <v>70</v>
@@ -4251,9 +3994,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="8">
         <v>70</v>
@@ -4289,9 +4032,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="8">
         <v>73</v>
@@ -4327,9 +4070,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8">
         <v>90</v>
@@ -4365,9 +4108,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="8">
         <v>70</v>
@@ -4403,9 +4146,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8">
         <v>70</v>
@@ -4441,9 +4184,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="8">
         <v>70</v>
@@ -4479,9 +4222,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="8">
         <v>110</v>
@@ -4517,9 +4260,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8">
         <v>70</v>
@@ -4555,9 +4298,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -4593,9 +4336,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4631,9 +4374,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4669,9 +4412,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B18" s="8">
         <f>B12</f>
@@ -4710,9 +4453,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="8">
         <v>70</v>
@@ -4748,9 +4491,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="8">
         <v>70</v>

</xml_diff>

<commit_message>
fix to databases names
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -54,15 +54,9 @@
     <t>type_shade</t>
   </si>
   <si>
-    <t>Ve_lps</t>
-  </si>
-  <si>
     <t>Ths_set_C</t>
   </si>
   <si>
-    <t>X_ghp</t>
-  </si>
-  <si>
     <t>Ea_Wm2</t>
   </si>
   <si>
@@ -72,18 +66,9 @@
     <t>Epro_Wm2</t>
   </si>
   <si>
-    <t>Qs_Wp</t>
-  </si>
-  <si>
     <t>Tcs_set_C</t>
   </si>
   <si>
-    <t>Vww_lpd</t>
-  </si>
-  <si>
-    <t>Vw_lpd</t>
-  </si>
-  <si>
     <t>MULTI_RES</t>
   </si>
   <si>
@@ -259,6 +244,21 @@
   </si>
   <si>
     <t>Occ_m2pax</t>
+  </si>
+  <si>
+    <t>Vw_lpdpax</t>
+  </si>
+  <si>
+    <t>Vww_lpdpax</t>
+  </si>
+  <si>
+    <t>X_ghpax</t>
+  </si>
+  <si>
+    <t>Qs_Wpax</t>
+  </si>
+  <si>
+    <t>Ve_lpspax</t>
   </si>
 </sst>
 </file>
@@ -1167,55 +1167,55 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>6</v>
@@ -1223,16 +1223,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3">
         <v>0.9</v>
@@ -1259,37 +1259,37 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="T2" s="11"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3">
         <v>0.9</v>
@@ -1316,36 +1316,36 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3">
         <v>0.9</v>
@@ -1372,36 +1372,36 @@
         <v>0.35</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
@@ -1428,36 +1428,36 @@
         <v>0.59</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3">
         <v>0.9</v>
@@ -1484,36 +1484,36 @@
         <v>0.59</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3">
         <v>0.9</v>
@@ -1540,36 +1540,36 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3">
         <v>0.9</v>
@@ -1596,36 +1596,36 @@
         <v>0.59</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3">
         <v>0.9</v>
@@ -1652,36 +1652,36 @@
         <v>0.1</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3">
         <v>0.9</v>
@@ -1708,36 +1708,36 @@
         <v>0.35</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3">
         <v>0.9</v>
@@ -1764,36 +1764,36 @@
         <v>0.35</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3">
         <v>0.9</v>
@@ -1820,36 +1820,36 @@
         <v>0.35</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3">
         <v>0.9</v>
@@ -1876,36 +1876,36 @@
         <v>0.35</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3">
         <v>0.9</v>
@@ -1932,36 +1932,36 @@
         <v>0.35</v>
       </c>
       <c r="M14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R14" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3">
         <v>0.9</v>
@@ -1988,36 +1988,36 @@
         <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3">
         <v>0.9</v>
@@ -2044,36 +2044,36 @@
         <v>0.5</v>
       </c>
       <c r="M16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="R16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3">
         <v>0.9</v>
@@ -2100,36 +2100,36 @@
         <v>0</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3">
         <v>0.9</v>
@@ -2156,36 +2156,36 @@
         <v>0.35</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3">
         <v>0.9</v>
@@ -2212,36 +2212,36 @@
         <v>0.35</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3">
         <v>0.9</v>
@@ -2268,22 +2268,22 @@
         <v>0.35</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2317,16 +2317,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2338,501 +2338,501 @@
         <v>3</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -2866,16 +2866,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2890,558 +2890,558 @@
         <v>5</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -3460,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,30 +3480,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="8">
         <v>28</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8">
         <v>28</v>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8">
         <v>24</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="8">
         <v>24</v>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8">
         <v>24</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>24</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8">
         <v>24</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="8">
         <v>24</v>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="8">
         <v>24</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="8">
         <v>50</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="8">
         <v>24</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="8">
         <v>50</v>
@@ -3894,7 +3894,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8">
         <v>-5</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" s="8">
         <v>24</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" s="8">
         <v>24</v>
@@ -4007,8 +4007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,45 +4031,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="8">
         <v>35</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8">
         <v>60</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8">
         <v>23</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8">
         <v>6</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8">
         <v>2.7</v>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="8">
         <v>13</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10" s="8">
         <v>19</v>
@@ -4438,7 +4438,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="8">
         <v>4</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8">
         <v>19</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="8">
         <v>9</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="8">
         <v>20</v>
@@ -4602,7 +4602,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" s="8">
         <v>20</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" s="8">
         <v>10</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" s="8">
         <v>9</v>

</xml_diff>

<commit_message>
creating `Hs_ag` and `Hs_bg` for internal gains proportions in RC-model
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="77">
   <si>
     <t>Code</t>
   </si>
   <si>
-    <t>Hs</t>
-  </si>
-  <si>
     <t>type_hs</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>RH_max_pc</t>
+  </si>
+  <si>
+    <t>Hs_ag</t>
+  </si>
+  <si>
+    <t>Hs_bg</t>
   </si>
 </sst>
 </file>
@@ -1141,98 +1144,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
-    <col min="5" max="7" width="7.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="10.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.73046875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.73046875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" style="4" customWidth="1"/>
+    <col min="5" max="8" width="7.1328125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10.86328125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="12.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3">
         <v>0.9</v>
@@ -1241,13 +1247,13 @@
         <v>0.25</v>
       </c>
       <c r="G2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
       <c r="I2" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="J2" s="3">
         <v>0.28999999999999998</v>
@@ -1258,38 +1264,41 @@
       <c r="L2" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3">
         <v>0.9</v>
@@ -1298,13 +1307,13 @@
         <v>0.25</v>
       </c>
       <c r="G3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
       <c r="I3" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="J3" s="3">
         <v>0.28999999999999998</v>
@@ -1315,37 +1324,40 @@
       <c r="L3" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3">
         <v>0.9</v>
@@ -1354,13 +1366,13 @@
         <v>0.84</v>
       </c>
       <c r="G4" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
       <c r="I4" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
         <v>0.35</v>
@@ -1371,37 +1383,40 @@
       <c r="L4" s="3">
         <v>0.35</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>45</v>
+      <c r="M4" s="3">
+        <v>0.35</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
@@ -1410,13 +1425,13 @@
         <v>0.84</v>
       </c>
       <c r="G5" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
       <c r="I5" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J5" s="3">
         <v>0.59</v>
@@ -1427,37 +1442,40 @@
       <c r="L5" s="3">
         <v>0.59</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>45</v>
+      <c r="M5" s="3">
+        <v>0.59</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3">
         <v>0.9</v>
@@ -1466,13 +1484,13 @@
         <v>0.84</v>
       </c>
       <c r="G6" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
       <c r="I6" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J6" s="3">
         <v>0.59</v>
@@ -1483,37 +1501,40 @@
       <c r="L6" s="3">
         <v>0.59</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>45</v>
+      <c r="M6" s="3">
+        <v>0.59</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3">
         <v>0.9</v>
@@ -1522,11 +1543,11 @@
         <v>0.84</v>
       </c>
       <c r="G7" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
@@ -1539,37 +1560,40 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>45</v>
+      <c r="M7" s="3">
+        <v>0</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3">
         <v>0.9</v>
@@ -1578,13 +1602,13 @@
         <v>0.84</v>
       </c>
       <c r="G8" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
       <c r="I8" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J8" s="3">
         <v>0.59</v>
@@ -1595,37 +1619,40 @@
       <c r="L8" s="3">
         <v>0.59</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>45</v>
+      <c r="M8" s="3">
+        <v>0.59</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3">
         <v>0.9</v>
@@ -1634,13 +1661,13 @@
         <v>0.7</v>
       </c>
       <c r="G9" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
       <c r="I9" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3">
         <v>0.1</v>
@@ -1651,37 +1678,40 @@
       <c r="L9" s="3">
         <v>0.1</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>45</v>
+      <c r="M9" s="3">
+        <v>0.1</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3">
         <v>0.9</v>
@@ -1690,13 +1720,13 @@
         <v>0.67</v>
       </c>
       <c r="G10" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
       <c r="I10" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J10" s="3">
         <v>0.35</v>
@@ -1707,37 +1737,40 @@
       <c r="L10" s="3">
         <v>0.35</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>45</v>
+      <c r="M10" s="3">
+        <v>0.35</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3">
         <v>0.9</v>
@@ -1746,13 +1779,13 @@
         <v>0.67</v>
       </c>
       <c r="G11" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
       <c r="I11" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J11" s="3">
         <v>0.35</v>
@@ -1763,37 +1796,40 @@
       <c r="L11" s="3">
         <v>0.35</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>45</v>
+      <c r="M11" s="3">
+        <v>0.35</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3">
         <v>0.9</v>
@@ -1802,13 +1838,13 @@
         <v>0.84</v>
       </c>
       <c r="G12" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="H12" s="3">
         <v>1</v>
       </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
       <c r="I12" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J12" s="3">
         <v>0.35</v>
@@ -1819,37 +1855,40 @@
       <c r="L12" s="3">
         <v>0.35</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>45</v>
+      <c r="M12" s="3">
+        <v>0.35</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3">
         <v>0.9</v>
@@ -1858,13 +1897,13 @@
         <v>0.67</v>
       </c>
       <c r="G13" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
       <c r="I13" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3">
         <v>0.35</v>
@@ -1875,37 +1914,40 @@
       <c r="L13" s="3">
         <v>0.35</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>45</v>
+      <c r="M13" s="3">
+        <v>0.35</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3">
         <v>0.9</v>
@@ -1914,13 +1956,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
       <c r="I14" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3">
         <v>0.35</v>
@@ -1931,37 +1973,40 @@
       <c r="L14" s="3">
         <v>0.35</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>45</v>
+      <c r="M14" s="3">
+        <v>0.35</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3">
         <v>0.9</v>
@@ -1973,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
@@ -1987,37 +2032,40 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>45</v>
+      <c r="M15" s="3">
+        <v>0</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3">
         <v>0.9</v>
@@ -2026,13 +2074,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
         <v>0.5</v>
@@ -2043,37 +2091,40 @@
       <c r="L16" s="3">
         <v>0.5</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="R16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3">
         <v>0.9</v>
@@ -2085,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
         <v>0</v>
@@ -2099,37 +2150,40 @@
       <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>45</v>
+      <c r="M17" s="3">
+        <v>0</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3">
         <v>0.9</v>
@@ -2138,13 +2192,13 @@
         <v>0.67</v>
       </c>
       <c r="G18" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H18" s="3">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
       <c r="I18" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J18" s="3">
         <v>0.35</v>
@@ -2155,37 +2209,40 @@
       <c r="L18" s="3">
         <v>0.35</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>45</v>
+      <c r="M18" s="3">
+        <v>0.35</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3">
         <v>0.9</v>
@@ -2194,13 +2251,13 @@
         <v>0.67</v>
       </c>
       <c r="G19" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
       <c r="I19" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J19" s="3">
         <v>0.35</v>
@@ -2211,37 +2268,40 @@
       <c r="L19" s="3">
         <v>0.35</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>45</v>
+      <c r="M19" s="3">
+        <v>0.35</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="3">
         <v>0.9</v>
@@ -2250,13 +2310,13 @@
         <v>0.67</v>
       </c>
       <c r="G20" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
       <c r="I20" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
         <v>0.35</v>
@@ -2267,23 +2327,26 @@
       <c r="L20" s="3">
         <v>0.35</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>45</v>
+      <c r="M20" s="3">
+        <v>0.35</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2303,539 +2366,539 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="4"/>
-    <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="4"/>
-    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" style="4"/>
+    <col min="6" max="6" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" style="4"/>
+    <col min="8" max="8" width="8.86328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="H10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="H13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="H17" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="H18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H20" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -2851,600 +2914,600 @@
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.1328125" style="4"/>
+    <col min="7" max="7" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="I1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="G18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="G20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -3460,50 +3523,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.73046875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="8">
         <v>28</v>
@@ -3527,9 +3590,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <v>28</v>
@@ -3553,9 +3616,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>24</v>
@@ -3579,9 +3642,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
         <v>24</v>
@@ -3605,9 +3668,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8">
         <v>24</v>
@@ -3631,9 +3694,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>24</v>
@@ -3657,9 +3720,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8">
         <v>24</v>
@@ -3684,9 +3747,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8">
         <v>24</v>
@@ -3710,9 +3773,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -3736,9 +3799,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -3762,9 +3825,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -3788,9 +3851,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>24</v>
@@ -3814,9 +3877,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>50</v>
@@ -3840,9 +3903,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>24</v>
@@ -3866,9 +3929,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>50</v>
@@ -3892,9 +3955,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>-5</v>
@@ -3918,9 +3981,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="8">
         <v>24</v>
@@ -3945,9 +4008,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -3971,9 +4034,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8">
         <v>24</v>
@@ -4011,65 +4074,65 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="8.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.73046875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="8">
         <v>35</v>
@@ -4108,9 +4171,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <v>60</v>
@@ -4149,9 +4212,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>23</v>
@@ -4190,9 +4253,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
@@ -4231,9 +4294,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8">
         <v>6</v>
@@ -4272,9 +4335,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4313,9 +4376,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8">
         <v>2.7</v>
@@ -4354,9 +4417,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8">
         <v>13</v>
@@ -4395,9 +4458,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="8">
         <v>19</v>
@@ -4436,9 +4499,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>4</v>
@@ -4477,9 +4540,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>19</v>
@@ -4518,9 +4581,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>9</v>
@@ -4559,9 +4622,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>20</v>
@@ -4600,9 +4663,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -4641,9 +4704,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4682,9 +4745,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4723,9 +4786,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="8">
         <v>20</v>
@@ -4767,9 +4830,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8">
         <v>10</v>
@@ -4808,9 +4871,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8">
         <v>9</v>

</xml_diff>

<commit_message>
fixes to new seasonality
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="83">
   <si>
     <t>Code</t>
   </si>
@@ -259,6 +259,27 @@
   </si>
   <si>
     <t>RH_max_pc</t>
+  </si>
+  <si>
+    <t>01|01</t>
+  </si>
+  <si>
+    <t>00|00</t>
+  </si>
+  <si>
+    <t>31|12</t>
+  </si>
+  <si>
+    <t>heat_starts</t>
+  </si>
+  <si>
+    <t>heat_ends</t>
+  </si>
+  <si>
+    <t>cool_starts</t>
+  </si>
+  <si>
+    <t>cool_ends</t>
   </si>
 </sst>
 </file>
@@ -785,7 +806,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,6 +839,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2299,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -2848,10 +2872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,15 +2883,19 @@
     <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="4"/>
     <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>43</v>
       </c>
@@ -2895,8 +2923,20 @@
       <c r="I1" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -2924,8 +2964,20 @@
       <c r="I2" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -2953,8 +3005,20 @@
       <c r="I3" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -2982,8 +3046,20 @@
       <c r="I4" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -3011,8 +3087,20 @@
       <c r="I5" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -3040,8 +3128,20 @@
       <c r="I6" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
@@ -3069,8 +3169,20 @@
       <c r="I7" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -3098,8 +3210,20 @@
       <c r="I8" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -3127,8 +3251,20 @@
       <c r="I9" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
@@ -3156,8 +3292,20 @@
       <c r="I10" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -3185,8 +3333,20 @@
       <c r="I11" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -3214,8 +3374,20 @@
       <c r="I12" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -3243,8 +3415,20 @@
       <c r="I13" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -3272,8 +3456,20 @@
       <c r="I14" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
@@ -3301,8 +3497,20 @@
       <c r="I15" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -3330,8 +3538,20 @@
       <c r="I16" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -3359,8 +3579,20 @@
       <c r="I17" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -3388,8 +3620,20 @@
       <c r="I18" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
@@ -3417,8 +3661,20 @@
       <c r="I19" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>36</v>
       </c>
@@ -3445,6 +3701,18 @@
       </c>
       <c r="I20" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update databases to reflect recent changes in Hs_ag and Hs_bg
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/construction_properties.xlsx
+++ b/cea/databases/SG/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="84">
   <si>
     <t>Code</t>
   </si>
   <si>
-    <t>Hs</t>
-  </si>
-  <si>
     <t>type_hs</t>
   </si>
   <si>
@@ -280,6 +277,12 @@
   </si>
   <si>
     <t>cool_ends</t>
+  </si>
+  <si>
+    <t>Hs_ag</t>
+  </si>
+  <si>
+    <t>Hs_bg</t>
   </si>
 </sst>
 </file>
@@ -1165,13 +1168,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,83 +1183,86 @@
     <col min="2" max="2" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
-    <col min="5" max="7" width="7.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="10.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="8" width="7.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3">
         <v>0.9</v>
@@ -1264,14 +1270,14 @@
       <c r="F2" s="3">
         <v>0.25</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
       <c r="I2" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="J2" s="3">
         <v>0.28999999999999998</v>
@@ -1282,38 +1288,41 @@
       <c r="L2" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3">
         <v>0.9</v>
@@ -1321,14 +1330,14 @@
       <c r="F3" s="3">
         <v>0.25</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
       <c r="I3" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="J3" s="3">
         <v>0.28999999999999998</v>
@@ -1339,37 +1348,40 @@
       <c r="L3" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3">
         <v>0.9</v>
@@ -1377,14 +1389,14 @@
       <c r="F4" s="3">
         <v>0.84</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
       <c r="I4" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
         <v>0.35</v>
@@ -1395,37 +1407,40 @@
       <c r="L4" s="3">
         <v>0.35</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>45</v>
+      <c r="M4" s="3">
+        <v>0.35</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
@@ -1433,14 +1448,14 @@
       <c r="F5" s="3">
         <v>0.84</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
       <c r="I5" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J5" s="3">
         <v>0.59</v>
@@ -1451,37 +1466,40 @@
       <c r="L5" s="3">
         <v>0.59</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>45</v>
+      <c r="M5" s="3">
+        <v>0.59</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3">
         <v>0.9</v>
@@ -1489,14 +1507,14 @@
       <c r="F6" s="3">
         <v>0.84</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
       <c r="I6" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J6" s="3">
         <v>0.59</v>
@@ -1507,37 +1525,40 @@
       <c r="L6" s="3">
         <v>0.59</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>45</v>
+      <c r="M6" s="3">
+        <v>0.59</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3">
         <v>0.9</v>
@@ -1545,12 +1566,12 @@
       <c r="F7" s="3">
         <v>0.84</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
@@ -1563,37 +1584,40 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>45</v>
+      <c r="M7" s="3">
+        <v>0</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3">
         <v>0.9</v>
@@ -1601,14 +1625,14 @@
       <c r="F8" s="3">
         <v>0.84</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
       <c r="I8" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="J8" s="3">
         <v>0.59</v>
@@ -1619,37 +1643,40 @@
       <c r="L8" s="3">
         <v>0.59</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>45</v>
+      <c r="M8" s="3">
+        <v>0.59</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3">
         <v>0.9</v>
@@ -1657,14 +1684,14 @@
       <c r="F9" s="3">
         <v>0.7</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
       <c r="I9" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3">
         <v>0.1</v>
@@ -1675,37 +1702,40 @@
       <c r="L9" s="3">
         <v>0.1</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>45</v>
+      <c r="M9" s="3">
+        <v>0.1</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3">
         <v>0.9</v>
@@ -1713,14 +1743,14 @@
       <c r="F10" s="3">
         <v>0.67</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
       <c r="I10" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J10" s="3">
         <v>0.35</v>
@@ -1731,37 +1761,40 @@
       <c r="L10" s="3">
         <v>0.35</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>45</v>
+      <c r="M10" s="3">
+        <v>0.35</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3">
         <v>0.9</v>
@@ -1769,14 +1802,14 @@
       <c r="F11" s="3">
         <v>0.67</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
       <c r="I11" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J11" s="3">
         <v>0.35</v>
@@ -1787,37 +1820,40 @@
       <c r="L11" s="3">
         <v>0.35</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>45</v>
+      <c r="M11" s="3">
+        <v>0.35</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3">
         <v>0.9</v>
@@ -1825,14 +1861,14 @@
       <c r="F12" s="3">
         <v>0.84</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
         <v>1</v>
       </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
       <c r="I12" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J12" s="3">
         <v>0.35</v>
@@ -1843,37 +1879,40 @@
       <c r="L12" s="3">
         <v>0.35</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>45</v>
+      <c r="M12" s="3">
+        <v>0.35</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3">
         <v>0.9</v>
@@ -1881,14 +1920,14 @@
       <c r="F13" s="3">
         <v>0.67</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
       <c r="I13" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3">
         <v>0.35</v>
@@ -1899,37 +1938,40 @@
       <c r="L13" s="3">
         <v>0.35</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>45</v>
+      <c r="M13" s="3">
+        <v>0.35</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3">
         <v>0.9</v>
@@ -1937,14 +1979,14 @@
       <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
       <c r="I14" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3">
         <v>0.35</v>
@@ -1955,37 +1997,40 @@
       <c r="L14" s="3">
         <v>0.35</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>45</v>
+      <c r="M14" s="3">
+        <v>0.35</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3">
         <v>0.9</v>
@@ -1993,12 +2038,12 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
         <v>1</v>
       </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
@@ -2011,37 +2056,40 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>45</v>
+      <c r="M15" s="3">
+        <v>0</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3">
         <v>0.9</v>
@@ -2049,14 +2097,14 @@
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="3">
-        <v>1</v>
+      <c r="G16" s="8">
+        <v>0</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
         <v>0.5</v>
@@ -2067,37 +2115,40 @@
       <c r="L16" s="3">
         <v>0.5</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="R16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3">
         <v>0.9</v>
@@ -2105,12 +2156,12 @@
       <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
       <c r="I17" s="3">
         <v>0</v>
       </c>
@@ -2123,37 +2174,40 @@
       <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>45</v>
+      <c r="M17" s="3">
+        <v>0</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3">
         <v>0.9</v>
@@ -2161,14 +2215,14 @@
       <c r="F18" s="3">
         <v>0.67</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
       <c r="I18" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J18" s="3">
         <v>0.35</v>
@@ -2179,37 +2233,40 @@
       <c r="L18" s="3">
         <v>0.35</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>45</v>
+      <c r="M18" s="3">
+        <v>0.35</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3">
         <v>0.9</v>
@@ -2217,14 +2274,14 @@
       <c r="F19" s="3">
         <v>0.67</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
       <c r="I19" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J19" s="3">
         <v>0.35</v>
@@ -2235,37 +2292,40 @@
       <c r="L19" s="3">
         <v>0.35</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>45</v>
+      <c r="M19" s="3">
+        <v>0.35</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="3">
         <v>0.9</v>
@@ -2273,14 +2333,14 @@
       <c r="F20" s="3">
         <v>0.67</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
       <c r="I20" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
         <v>0.35</v>
@@ -2291,23 +2351,26 @@
       <c r="L20" s="3">
         <v>0.35</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>45</v>
+      <c r="M20" s="3">
+        <v>0.35</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2341,522 +2404,522 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -2874,7 +2937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -2897,822 +2960,822 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -3751,30 +3814,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="8">
         <v>28</v>
@@ -3800,7 +3863,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <v>28</v>
@@ -3826,7 +3889,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>24</v>
@@ -3852,7 +3915,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
         <v>24</v>
@@ -3878,7 +3941,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8">
         <v>24</v>
@@ -3904,7 +3967,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>24</v>
@@ -3930,7 +3993,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8">
         <v>24</v>
@@ -3957,7 +4020,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8">
         <v>24</v>
@@ -3983,7 +4046,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -4009,7 +4072,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -4035,7 +4098,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -4061,7 +4124,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>24</v>
@@ -4087,7 +4150,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>50</v>
@@ -4113,7 +4176,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>24</v>
@@ -4139,7 +4202,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>50</v>
@@ -4165,7 +4228,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>-5</v>
@@ -4191,7 +4254,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="8">
         <v>24</v>
@@ -4218,7 +4281,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -4244,7 +4307,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8">
         <v>24</v>
@@ -4302,45 +4365,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="8">
         <v>35</v>
@@ -4381,7 +4444,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <v>60</v>
@@ -4422,7 +4485,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>23</v>
@@ -4463,7 +4526,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
@@ -4504,7 +4567,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8">
         <v>6</v>
@@ -4545,7 +4608,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4586,7 +4649,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8">
         <v>2.7</v>
@@ -4627,7 +4690,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8">
         <v>13</v>
@@ -4668,7 +4731,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="8">
         <v>19</v>
@@ -4709,7 +4772,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>4</v>
@@ -4750,7 +4813,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>19</v>
@@ -4791,7 +4854,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>9</v>
@@ -4832,7 +4895,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>20</v>
@@ -4873,7 +4936,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -4914,7 +4977,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4955,7 +5018,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4996,7 +5059,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="8">
         <v>20</v>
@@ -5040,7 +5103,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8">
         <v>10</v>
@@ -5081,7 +5144,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8">
         <v>9</v>

</xml_diff>